<commit_message>
correction max damage clinics
</commit_message>
<xml_diff>
--- a/data/infra_vulnerability_data.xlsx
+++ b/data/infra_vulnerability_data.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="flooding_curves" sheetId="2" r:id="rId1"/>
-    <sheet name="correction_without_reference_ye" sheetId="3" r:id="rId2"/>
+    <sheet name="correction_without_inflation" sheetId="3" r:id="rId2"/>
     <sheet name="correction_reference_year" sheetId="5" r:id="rId3"/>
     <sheet name="power_points" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="113">
   <si>
     <t>cable</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>STEP 2</t>
+  </si>
+  <si>
+    <t>Misschien toch aanpassen naar zelfde vulnerability curve for lines --&gt; in FEMA zeggen ze wel iets over cables (p360)</t>
   </si>
 </sst>
 </file>
@@ -1113,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ68"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1611,7 @@
         <v>148865.17338917882</v>
       </c>
       <c r="AA4" s="14">
-        <v>165200</v>
+        <v>658.46820000000002</v>
       </c>
       <c r="AB4" s="14">
         <v>658.46820000000002</v>
@@ -1737,7 +1740,7 @@
         <v>90112.090429284988</v>
       </c>
       <c r="AA5" s="14">
-        <v>123900</v>
+        <v>493.85115000000002</v>
       </c>
       <c r="AB5" s="14">
         <v>493.85115000000002</v>
@@ -1866,7 +1869,7 @@
         <v>270336.27128785499</v>
       </c>
       <c r="AA6" s="14">
-        <v>206500</v>
+        <v>823.08525000000009</v>
       </c>
       <c r="AB6" s="14">
         <v>823.08525000000009</v>
@@ -1918,6 +1921,9 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>112</v>
+      </c>
       <c r="T7" s="20"/>
       <c r="U7" s="20"/>
       <c r="V7" s="20"/>
@@ -4889,8 +4895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6236,11 +6242,11 @@
         <v>601.61101894314208</v>
       </c>
       <c r="E20" s="14">
-        <f>E3/$D$12</f>
+        <f t="shared" ref="E20:F22" si="1">E3/$D$12</f>
         <v>409240349.46149552</v>
       </c>
       <c r="F20" s="14">
-        <f>F3/$D$12</f>
+        <f t="shared" si="1"/>
         <v>29762934.506290585</v>
       </c>
       <c r="G20" s="14">
@@ -6288,23 +6294,23 @@
         <v>900</v>
       </c>
       <c r="S20" s="14">
-        <f t="shared" ref="S20:W20" si="1">S3*1000000/1000</f>
+        <f t="shared" ref="S20:W20" si="2">S3*1000000/1000</f>
         <v>600</v>
       </c>
       <c r="T20" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>250</v>
       </c>
       <c r="U20" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>225</v>
       </c>
       <c r="V20" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>175</v>
       </c>
       <c r="W20" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="X20" s="14">
@@ -6324,67 +6330,67 @@
         <v>639</v>
       </c>
       <c r="AB20" s="14">
-        <f t="shared" ref="AB20:AQ20" si="2">AB3</f>
+        <f t="shared" ref="AB20:AQ20" si="3">AB3</f>
         <v>639</v>
       </c>
       <c r="AC20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AD20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AE20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AF20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AG20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AH20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AI20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AJ20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AK20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AL20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AM20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AN20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AO20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AP20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
       <c r="AQ20" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>639</v>
       </c>
     </row>
@@ -6393,31 +6399,31 @@
         <v>30</v>
       </c>
       <c r="B21" s="14">
-        <f t="shared" ref="B21:D21" si="3">(B4/$D$10)/$D$13</f>
+        <f t="shared" ref="B21:D21" si="4">(B4/$D$10)/$D$13</f>
         <v>544.05763475197909</v>
       </c>
       <c r="C21" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>160.74430117672111</v>
       </c>
       <c r="D21" s="14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74.189677466178964</v>
       </c>
       <c r="E21" s="14">
-        <f>E4/$D$12</f>
+        <f t="shared" si="1"/>
         <v>111611004.39858969</v>
       </c>
       <c r="F21" s="14">
-        <f>F4/$D$12</f>
+        <f t="shared" si="1"/>
         <v>11161100.439858967</v>
       </c>
       <c r="G21" s="14">
-        <f t="shared" ref="G21:H21" si="4">G4/$D$16</f>
+        <f t="shared" ref="G21:H21" si="5">G4/$D$16</f>
         <v>37549.239520649426</v>
       </c>
       <c r="H21" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17907.472102454787</v>
       </c>
       <c r="I21" s="14">
@@ -6445,7 +6451,7 @@
         <v>407.25</v>
       </c>
       <c r="P21" s="14">
-        <f t="shared" ref="P21:P22" si="5">P4/$D$12</f>
+        <f t="shared" ref="P21:P22" si="6">P4/$D$12</f>
         <v>66966602.639153808</v>
       </c>
       <c r="Q21" s="14">
@@ -6457,23 +6463,23 @@
         <v>675</v>
       </c>
       <c r="S21" s="14">
-        <f t="shared" ref="S21:W21" si="6">S20*0.75</f>
+        <f t="shared" ref="S21:W21" si="7">S20*0.75</f>
         <v>450</v>
       </c>
       <c r="T21" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>187.5</v>
       </c>
       <c r="U21" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>168.75</v>
       </c>
       <c r="V21" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>131.25</v>
       </c>
       <c r="W21" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>56.25</v>
       </c>
       <c r="X21" s="14">
@@ -6493,67 +6499,67 @@
         <v>479.25</v>
       </c>
       <c r="AB21" s="14">
-        <f t="shared" ref="AB21:AQ21" si="7">AB20*0.75</f>
+        <f t="shared" ref="AB21:AQ21" si="8">AB20*0.75</f>
         <v>479.25</v>
       </c>
       <c r="AC21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AD21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AE21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AF21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AG21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AH21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AI21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AJ21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AK21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AL21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AM21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AN21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AO21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AP21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AQ21" s="14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>479.25</v>
       </c>
       <c r="AR21" s="18"/>
@@ -6566,31 +6572,31 @@
         <v>94</v>
       </c>
       <c r="B22" s="14">
-        <f t="shared" ref="B22:D22" si="8">(B5/$D$10)/$D$13</f>
+        <f t="shared" ref="B22:D22" si="9">(B5/$D$10)/$D$13</f>
         <v>11375.750544814107</v>
       </c>
       <c r="C22" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2472.9892488726323</v>
       </c>
       <c r="D22" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1127.6830974859204</v>
       </c>
       <c r="E22" s="14">
-        <f>E5/$D$12</f>
+        <f t="shared" si="1"/>
         <v>558055021.99294841</v>
       </c>
       <c r="F22" s="14">
-        <f>F5/$D$12</f>
+        <f t="shared" si="1"/>
         <v>55805502.199294843</v>
       </c>
       <c r="G22" s="14">
-        <f t="shared" ref="G22:H22" si="9">G5/$D$16</f>
+        <f t="shared" ref="G22:H22" si="10">G5/$D$16</f>
         <v>725654.60087097215</v>
       </c>
       <c r="H22" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>59384.233709180466</v>
       </c>
       <c r="I22" s="14">
@@ -6618,7 +6624,7 @@
         <v>678.75</v>
       </c>
       <c r="P22" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>803599231.6698457</v>
       </c>
       <c r="Q22" s="14">
@@ -6630,23 +6636,23 @@
         <v>1125</v>
       </c>
       <c r="S22" s="14">
-        <f t="shared" ref="S22:W22" si="10">S20*1.25</f>
+        <f t="shared" ref="S22:W22" si="11">S20*1.25</f>
         <v>750</v>
       </c>
       <c r="T22" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>312.5</v>
       </c>
       <c r="U22" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>281.25</v>
       </c>
       <c r="V22" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>218.75</v>
       </c>
       <c r="W22" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>93.75</v>
       </c>
       <c r="X22" s="14">
@@ -6666,67 +6672,67 @@
         <v>798.75</v>
       </c>
       <c r="AB22" s="14">
-        <f t="shared" ref="AB22:AQ22" si="11">AB20*1.25</f>
+        <f t="shared" ref="AB22:AQ22" si="12">AB20*1.25</f>
         <v>798.75</v>
       </c>
       <c r="AC22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AD22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AE22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AF22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AG22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AH22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AI22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AJ22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AK22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AL22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AM22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AN22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AO22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AP22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AQ22" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>798.75</v>
       </c>
       <c r="AR22" s="18"/>
@@ -6764,8 +6770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7979,27 +7985,27 @@
         <v>843342.20000000007</v>
       </c>
       <c r="R16" s="73">
-        <f>R3</f>
+        <f t="shared" ref="R16:W18" si="1">R3</f>
         <v>0.9</v>
       </c>
       <c r="S16" s="73">
-        <f>S3</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="T16" s="73">
-        <f>T3</f>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="U16" s="73">
-        <f>U3</f>
+        <f t="shared" si="1"/>
         <v>0.22500000000000001</v>
       </c>
       <c r="V16" s="73">
-        <f>V3</f>
+        <f t="shared" si="1"/>
         <v>0.17499999999999999</v>
       </c>
       <c r="W16" s="73">
-        <f>W3</f>
+        <f t="shared" si="1"/>
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="X16" s="72">
@@ -8019,67 +8025,67 @@
         <v>658.46820000000002</v>
       </c>
       <c r="AB16" s="72">
-        <f t="shared" ref="AB16:AQ16" si="1">AB3*((AB15/100)+1)</f>
+        <f t="shared" ref="AB16:AQ16" si="2">AB3*((AB15/100)+1)</f>
         <v>658.46820000000002</v>
       </c>
       <c r="AC16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AD16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AE16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AF16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AG16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AH16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AI16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AJ16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AK16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AL16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AM16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AN16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AO16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AP16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AQ16" s="72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>658.46820000000002</v>
       </c>
     </row>
@@ -8144,27 +8150,27 @@
         <v>n/a</v>
       </c>
       <c r="R17" s="73" t="str">
-        <f>R4</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="S17" s="73" t="str">
-        <f>S4</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="T17" s="73" t="str">
-        <f>T4</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="U17" s="73" t="str">
-        <f>U4</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="V17" s="73" t="str">
-        <f>V4</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="W17" s="73" t="str">
-        <f>W4</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="X17" s="73" t="str">
@@ -8290,27 +8296,27 @@
         <v>n/a</v>
       </c>
       <c r="R18" s="73" t="str">
-        <f>R5</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="S18" s="73" t="str">
-        <f>S5</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="T18" s="73" t="str">
-        <f>T5</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="U18" s="73" t="str">
-        <f>U5</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="V18" s="73" t="str">
-        <f>V5</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="W18" s="73" t="str">
-        <f>W5</f>
+        <f t="shared" si="1"/>
         <v>n/a</v>
       </c>
       <c r="X18" s="73" t="str">
@@ -8588,11 +8594,11 @@
         <v>5343.1358802289315</v>
       </c>
       <c r="C32" s="80">
-        <f t="shared" ref="C32:D32" si="2">(C16/$E$26)/$E$28</f>
+        <f t="shared" ref="C32:D32" si="3">(C16/$E$26)/$E$28</f>
         <v>1442.3968280514925</v>
       </c>
       <c r="D32" s="80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>800.94936103904399</v>
       </c>
       <c r="E32" s="80">
@@ -8600,31 +8606,31 @@
         <v>442420326.64431292</v>
       </c>
       <c r="F32" s="80">
-        <f t="shared" ref="F32:L32" si="3">F16/$E$28</f>
+        <f t="shared" ref="F32:L32" si="4">F16/$E$28</f>
         <v>32176023.755950026</v>
       </c>
       <c r="G32" s="80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>201757.75136692534</v>
       </c>
       <c r="H32" s="80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>35565.727007825037</v>
       </c>
       <c r="I32" s="80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>965280.7126785008</v>
       </c>
       <c r="J32" s="80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>482640.3563392504</v>
       </c>
       <c r="K32" s="80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1117312.4249253648</v>
       </c>
       <c r="L32" s="80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>197078145.50519392</v>
       </c>
       <c r="N32" s="72">
@@ -8648,23 +8654,23 @@
         <v>900</v>
       </c>
       <c r="S32" s="80">
-        <f t="shared" ref="S32:W32" si="4">S16*1000000/1000</f>
+        <f t="shared" ref="S32:W32" si="5">S16*1000000/1000</f>
         <v>600</v>
       </c>
       <c r="T32" s="80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>250</v>
       </c>
       <c r="U32" s="80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>225</v>
       </c>
       <c r="V32" s="80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="W32" s="80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="X32" s="80">
@@ -8680,71 +8686,71 @@
         <v>148865.17338917882</v>
       </c>
       <c r="AA32" s="80">
-        <f>Z16</f>
-        <v>165200</v>
+        <f>AA16</f>
+        <v>658.46820000000002</v>
       </c>
       <c r="AB32" s="80">
-        <f t="shared" ref="AB32:AQ32" si="5">AA16</f>
+        <f t="shared" ref="AA32:AQ32" si="6">AA16</f>
         <v>658.46820000000002</v>
       </c>
       <c r="AC32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AD32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AE32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AF32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AG32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AH32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AI32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AJ32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AK32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AL32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AM32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AN32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AO32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AP32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
       <c r="AQ32" s="80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>658.46820000000002</v>
       </c>
     </row>
@@ -8753,31 +8759,31 @@
         <v>30</v>
       </c>
       <c r="B33" s="80">
-        <f t="shared" ref="B33:D34" si="6">(B17/$E$26)/$E$28</f>
+        <f t="shared" ref="B33:D34" si="7">(B17/$E$26)/$E$28</f>
         <v>724.32618619339962</v>
       </c>
       <c r="C33" s="80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>214.00546410259537</v>
       </c>
       <c r="D33" s="80">
-        <f t="shared" si="6"/>
+        <f>(D17/$E$26)/$E$28</f>
         <v>98.771752662736318</v>
       </c>
       <c r="E33" s="80">
-        <f t="shared" ref="E33:L34" si="7">E17/$E$28</f>
+        <f t="shared" ref="E33:L34" si="8">E17/$E$28</f>
         <v>120660089.0848126</v>
       </c>
       <c r="F33" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12066008.908481261</v>
       </c>
       <c r="G33" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>35488.851782732541</v>
       </c>
       <c r="H33" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>16924.860033395544</v>
       </c>
       <c r="I33" s="80">
@@ -8789,11 +8795,11 @@
         <v>361980.26725443779</v>
       </c>
       <c r="K33" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>36198.026725443779</v>
       </c>
       <c r="L33" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>36198026.72544378</v>
       </c>
       <c r="N33" s="72">
@@ -8805,7 +8811,7 @@
         <v>419.65755000000001</v>
       </c>
       <c r="P33" s="80">
-        <f t="shared" ref="P33:P34" si="8">P17/$E$28</f>
+        <f t="shared" ref="P33:P34" si="9">P17/$E$28</f>
         <v>72396053.450887561</v>
       </c>
       <c r="Q33" s="80">
@@ -8817,23 +8823,23 @@
         <v>675</v>
       </c>
       <c r="S33" s="80">
-        <f t="shared" ref="S33:W33" si="9">S32*0.75</f>
+        <f t="shared" ref="S33:W33" si="10">S32*0.75</f>
         <v>450</v>
       </c>
       <c r="T33" s="80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>187.5</v>
       </c>
       <c r="U33" s="80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>168.75</v>
       </c>
       <c r="V33" s="80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>131.25</v>
       </c>
       <c r="W33" s="80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>56.25</v>
       </c>
       <c r="X33" s="80">
@@ -8849,71 +8855,71 @@
         <v>90112.090429284988</v>
       </c>
       <c r="AA33" s="80">
-        <f>AA32*0.75</f>
-        <v>123900</v>
+        <f t="shared" ref="AA33" si="11">AA32*0.75</f>
+        <v>493.85115000000002</v>
       </c>
       <c r="AB33" s="80">
-        <f t="shared" ref="AB33:AQ33" si="10">AB32*0.75</f>
+        <f t="shared" ref="AB33:AQ33" si="12">AB32*0.75</f>
         <v>493.85115000000002</v>
       </c>
       <c r="AC33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AD33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AE33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AF33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AG33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AH33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AI33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AJ33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AK33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AL33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AM33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AN33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AO33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AP33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
       <c r="AQ33" s="80">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>493.85115000000002</v>
       </c>
     </row>
@@ -8922,31 +8928,31 @@
         <v>94</v>
       </c>
       <c r="B34" s="80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15145.002074952903</v>
       </c>
       <c r="C34" s="80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3292.391755424544</v>
       </c>
       <c r="D34" s="80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1501.330640473592</v>
       </c>
       <c r="E34" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>603300445.42406297</v>
       </c>
       <c r="F34" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>60330044.542406298</v>
       </c>
       <c r="G34" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>685836.75473922014</v>
       </c>
       <c r="H34" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>56125.724388566938</v>
       </c>
       <c r="I34" s="80">
@@ -8958,11 +8964,11 @@
         <v>603300.44542406301</v>
       </c>
       <c r="K34" s="80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1809901.3362721889</v>
       </c>
       <c r="L34" s="80">
-        <f t="shared" si="7"/>
+        <f>L18/$E$28</f>
         <v>434376320.70532537</v>
       </c>
       <c r="N34" s="72">
@@ -8974,7 +8980,7 @@
         <v>699.42925000000002</v>
       </c>
       <c r="P34" s="80">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>868752641.41065073</v>
       </c>
       <c r="Q34" s="80">
@@ -8986,23 +8992,23 @@
         <v>1125</v>
       </c>
       <c r="S34" s="80">
-        <f t="shared" ref="S34:W34" si="11">S32*1.25</f>
+        <f t="shared" ref="S34:W34" si="13">S32*1.25</f>
         <v>750</v>
       </c>
       <c r="T34" s="80">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>312.5</v>
       </c>
       <c r="U34" s="80">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>281.25</v>
       </c>
       <c r="V34" s="80">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>218.75</v>
       </c>
       <c r="W34" s="80">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>93.75</v>
       </c>
       <c r="X34" s="80">
@@ -9018,71 +9024,71 @@
         <v>270336.27128785499</v>
       </c>
       <c r="AA34" s="80">
-        <f>AA32*1.25</f>
-        <v>206500</v>
+        <f t="shared" ref="AA34" si="14">AA32*1.25</f>
+        <v>823.08525000000009</v>
       </c>
       <c r="AB34" s="80">
-        <f t="shared" ref="AB34:AQ34" si="12">AB32*1.25</f>
+        <f t="shared" ref="AB34:AQ34" si="15">AB32*1.25</f>
         <v>823.08525000000009</v>
       </c>
       <c r="AC34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AD34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AE34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AF34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AG34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AH34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AI34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AJ34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AK34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AL34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AM34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AN34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AO34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AP34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
       <c r="AQ34" s="80">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>823.08525000000009</v>
       </c>
     </row>
@@ -9099,8 +9105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correction fragility data railway
</commit_message>
<xml_diff>
--- a/data/infra_vulnerability_data.xlsx
+++ b/data/infra_vulnerability_data.xlsx
@@ -1117,7 +1117,7 @@
   <dimension ref="A1:AQ68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,6 +2118,7 @@
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
       <c r="Q11" s="24">
+        <f>11700/702200</f>
         <v>1.6661919681002564E-2</v>
       </c>
       <c r="R11" s="16"/>
@@ -2175,8 +2176,8 @@
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
       <c r="Q12" s="24">
-        <f>135550/Q4</f>
-        <v>16.072953541278974</v>
+        <f>135550/702200</f>
+        <v>0.19303617203076046</v>
       </c>
       <c r="R12" s="16"/>
       <c r="S12" s="16"/>
@@ -8690,7 +8691,7 @@
         <v>658.46820000000002</v>
       </c>
       <c r="AB32" s="80">
-        <f t="shared" ref="AA32:AQ32" si="6">AA16</f>
+        <f t="shared" ref="AB32:AQ32" si="6">AA16</f>
         <v>658.46820000000002</v>
       </c>
       <c r="AC32" s="80">

</xml_diff>

<commit_message>
rename airports to aerodrome
</commit_message>
<xml_diff>
--- a/data/infra_vulnerability_data.xlsx
+++ b/data/infra_vulnerability_data.xlsx
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="180">
   <si>
     <t>cable</t>
   </si>
@@ -652,6 +652,9 @@
   </si>
   <si>
     <t>no - Huizinga already adjusted for this (+ also adjusted for depreciated value)</t>
+  </si>
+  <si>
+    <t>aerodrome</t>
   </si>
 </sst>
 </file>
@@ -2552,8 +2555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,7 +2657,7 @@
         <v>85</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>53</v>
+        <v>179</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
Rename aerodrome to airports
for consistency with other code
</commit_message>
<xml_diff>
--- a/data/infra_vulnerability_data.xlsx
+++ b/data/infra_vulnerability_data.xlsx
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="179">
   <si>
     <t>cable</t>
   </si>
@@ -652,9 +652,6 @@
   </si>
   <si>
     <t>no - Huizinga already adjusted for this (+ also adjusted for depreciated value)</t>
-  </si>
-  <si>
-    <t>aerodrome</t>
   </si>
 </sst>
 </file>
@@ -2556,7 +2553,7 @@
   <dimension ref="A1:AS68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,7 +2654,7 @@
         <v>85</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>179</v>
+        <v>53</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>146</v>

</xml_diff>

<commit_message>
latest code with fixed emilia romagna
</commit_message>
<xml_diff>
--- a/data/infra_vulnerability_data.xlsx
+++ b/data/infra_vulnerability_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snn490\surfdrive\My research articles\Article 2 multi-hazard analysis\Vulnerability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\labsdfs.labs.vu.nl\labsdfs\BETA-IVM-BAZIS\eks510\projects\gmhcira\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1245,7 +1245,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1551,7 +1551,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="16514559"/>
@@ -1613,7 +1613,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="16514975"/>
@@ -1655,7 +1655,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1685,7 +1685,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2552,38 +2552,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AP8" sqref="AP8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="11.7109375" style="82" customWidth="1"/>
-    <col min="27" max="27" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="11.6640625" style="82" customWidth="1"/>
+    <col min="27" max="27" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="45" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="45" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>34</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>27</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="str">
         <f>correction_reference_year!A47</f>
         <v>MaxDam</v>
@@ -3170,7 +3170,7 @@
         <v>658.46820000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="82" t="str">
         <f>correction_reference_year!A48</f>
         <v>LowerDam</v>
@@ -3352,7 +3352,7 @@
         <v>493.85115000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="82" t="str">
         <f>correction_reference_year!A49</f>
         <v>Upperdam</v>
@@ -3534,7 +3534,7 @@
         <v>823.08525000000009</v>
       </c>
     </row>
-    <row r="7" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>112</v>
       </c>
@@ -3563,7 +3563,7 @@
       <c r="AR7" s="20"/>
       <c r="AS7" s="20"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
       <c r="H8" s="17"/>
       <c r="I8" s="58"/>
       <c r="R8" s="19"/>
@@ -3573,7 +3573,7 @@
       <c r="V8" s="19"/>
       <c r="W8" s="19"/>
     </row>
-    <row r="9" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3585,7 +3585,7 @@
       <c r="V9" s="19"/>
       <c r="W9" s="19"/>
     </row>
-    <row r="10" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="AR11" s="16"/>
       <c r="AS11" s="16"/>
     </row>
-    <row r="12" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>20</v>
       </c>
@@ -3842,7 +3842,7 @@
       <c r="AR12" s="16"/>
       <c r="AS12" s="16"/>
     </row>
-    <row r="13" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18">
         <v>30</v>
       </c>
@@ -3924,7 +3924,7 @@
       <c r="AR13" s="16"/>
       <c r="AS13" s="16"/>
     </row>
-    <row r="14" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>50</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="15" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>60</v>
       </c>
@@ -4098,7 +4098,7 @@
       <c r="AR15" s="16"/>
       <c r="AS15" s="16"/>
     </row>
-    <row r="16" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18">
         <v>61</v>
       </c>
@@ -4180,7 +4180,7 @@
       <c r="AR16" s="16"/>
       <c r="AS16" s="16"/>
     </row>
-    <row r="17" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18">
         <v>91</v>
       </c>
@@ -4262,7 +4262,7 @@
       <c r="AR17" s="16"/>
       <c r="AS17" s="16"/>
     </row>
-    <row r="18" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>100</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="19" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18">
         <v>122</v>
       </c>
@@ -4457,7 +4457,7 @@
       <c r="AR19" s="26"/>
       <c r="AS19" s="26"/>
     </row>
-    <row r="20" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>140</v>
       </c>
@@ -4520,7 +4520,7 @@
       <c r="AR20" s="16"/>
       <c r="AS20" s="16"/>
     </row>
-    <row r="21" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>146</v>
       </c>
@@ -4581,7 +4581,7 @@
       <c r="AR21" s="16"/>
       <c r="AS21" s="16"/>
     </row>
-    <row r="22" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>150</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="23" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18">
         <v>152</v>
       </c>
@@ -4776,7 +4776,7 @@
       <c r="AR23" s="26"/>
       <c r="AS23" s="26"/>
     </row>
-    <row r="24" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
         <v>183</v>
       </c>
@@ -4858,7 +4858,7 @@
       <c r="AR24" s="26"/>
       <c r="AS24" s="26"/>
     </row>
-    <row r="25" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>200</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="26" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>212</v>
       </c>
@@ -5032,7 +5032,7 @@
       <c r="AR26" s="16"/>
       <c r="AS26" s="16"/>
     </row>
-    <row r="27" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18">
         <v>213</v>
       </c>
@@ -5114,7 +5114,7 @@
       <c r="AR27" s="16"/>
       <c r="AS27" s="16"/>
     </row>
-    <row r="28" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18">
         <v>244</v>
       </c>
@@ -5196,7 +5196,7 @@
       <c r="AR28" s="16"/>
       <c r="AS28" s="16"/>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>248</v>
       </c>
@@ -5257,7 +5257,7 @@
       <c r="AR29" s="16"/>
       <c r="AS29" s="16"/>
     </row>
-    <row r="30" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>250</v>
       </c>
@@ -5318,7 +5318,7 @@
       <c r="AR30" s="16"/>
       <c r="AS30" s="16"/>
     </row>
-    <row r="31" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18">
         <v>274</v>
       </c>
@@ -5400,7 +5400,7 @@
       <c r="AR31" s="16"/>
       <c r="AS31" s="16"/>
     </row>
-    <row r="32" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>300</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="33" spans="1:45" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:45" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18">
         <v>305</v>
       </c>
@@ -5594,7 +5594,7 @@
       <c r="AR33" s="26"/>
       <c r="AS33" s="26"/>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>329</v>
       </c>
@@ -5650,7 +5650,7 @@
       <c r="AR34" s="16"/>
       <c r="AS34" s="16"/>
     </row>
-    <row r="35" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>350</v>
       </c>
@@ -5706,7 +5706,7 @@
       <c r="AR35" s="16"/>
       <c r="AS35" s="16"/>
     </row>
-    <row r="36" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>400</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>402</v>
       </c>
@@ -5870,7 +5870,7 @@
       <c r="AR37" s="16"/>
       <c r="AS37" s="16"/>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>421</v>
       </c>
@@ -5926,7 +5926,7 @@
       <c r="AR38" s="16"/>
       <c r="AS38" s="16"/>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>450</v>
       </c>
@@ -5982,7 +5982,7 @@
       <c r="AR39" s="16"/>
       <c r="AS39" s="16"/>
     </row>
-    <row r="40" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>487</v>
       </c>
@@ -6038,7 +6038,7 @@
       <c r="AR40" s="16"/>
       <c r="AS40" s="16"/>
     </row>
-    <row r="41" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>500</v>
       </c>
@@ -6146,7 +6146,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="42" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>560</v>
       </c>
@@ -6202,7 +6202,7 @@
       <c r="AR42" s="16"/>
       <c r="AS42" s="16"/>
     </row>
-    <row r="43" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>600</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>627</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>628</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>715</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>779</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>782</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>877</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>999</v>
       </c>
@@ -6542,7 +6542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1003</v>
       </c>
@@ -6575,50 +6575,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
       <c r="F52" s="14"/>
       <c r="G52" s="14"/>
       <c r="AA52" s="19"/>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
       <c r="F53" s="15"/>
       <c r="G53" s="15"/>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
       <c r="F54" s="15"/>
       <c r="G54" s="15"/>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
       <c r="D57" s="15"/>
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
@@ -6626,7 +6626,7 @@
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
@@ -6634,7 +6634,7 @@
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
@@ -6643,7 +6643,7 @@
       <c r="G61" s="15"/>
       <c r="J61" s="18"/>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.3">
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
       <c r="E62" s="18"/>
@@ -6651,21 +6651,21 @@
       <c r="G62" s="15"/>
       <c r="J62" s="18"/>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D63" s="15"/>
       <c r="E63" s="18"/>
       <c r="F63" s="15"/>
       <c r="G63" s="15"/>
       <c r="J63" s="18"/>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.3">
       <c r="D64" s="15"/>
       <c r="E64" s="18"/>
       <c r="F64" s="15"/>
       <c r="G64" s="15"/>
       <c r="J64" s="18"/>
     </row>
-    <row r="65" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D65" s="15"/>
       <c r="E65" s="18"/>
       <c r="F65" s="15"/>
@@ -6675,17 +6675,17 @@
       <c r="R65" s="10"/>
       <c r="S65" s="10"/>
     </row>
-    <row r="66" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D66" s="15"/>
       <c r="E66" s="18"/>
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
       <c r="J66" s="18"/>
     </row>
-    <row r="67" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:19" x14ac:dyDescent="0.3">
       <c r="J67" s="18"/>
     </row>
-    <row r="68" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:19" x14ac:dyDescent="0.3">
       <c r="J68" s="18"/>
     </row>
   </sheetData>
@@ -6702,30 +6702,30 @@
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="12" style="18" customWidth="1"/>
-    <col min="20" max="22" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="43" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="43" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
@@ -6856,7 +6856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>27</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>29</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="4" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>30</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>31</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>58</v>
       </c>
@@ -7495,7 +7495,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -7623,7 +7623,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:43" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="X8" s="20"/>
       <c r="Y8" s="20"/>
       <c r="AA8" s="20"/>
@@ -7644,7 +7644,7 @@
       <c r="AP8" s="20"/>
       <c r="AQ8" s="20"/>
     </row>
-    <row r="9" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="44" t="s">
         <v>103</v>
       </c>
@@ -7673,7 +7673,7 @@
       <c r="AP9" s="20"/>
       <c r="AQ9" s="20"/>
     </row>
-    <row r="10" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="39"/>
       <c r="C10" s="19" t="s">
         <v>99</v>
@@ -7706,7 +7706,7 @@
       <c r="AP10" s="20"/>
       <c r="AQ10" s="20"/>
     </row>
-    <row r="11" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="39"/>
       <c r="C11" s="19" t="s">
         <v>101</v>
@@ -7737,7 +7737,7 @@
       <c r="AP11" s="20"/>
       <c r="AQ11" s="20"/>
     </row>
-    <row r="12" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="39"/>
       <c r="C12" s="19">
         <v>2001</v>
@@ -7768,7 +7768,7 @@
       <c r="AP12" s="20"/>
       <c r="AQ12" s="20"/>
     </row>
-    <row r="13" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="39"/>
       <c r="C13" s="19">
         <v>2006</v>
@@ -7799,7 +7799,7 @@
       <c r="AP13" s="20"/>
       <c r="AQ13" s="20"/>
     </row>
-    <row r="14" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="39"/>
       <c r="C14" s="19">
         <v>2015</v>
@@ -7831,7 +7831,7 @@
       <c r="AP14" s="20"/>
       <c r="AQ14" s="20"/>
     </row>
-    <row r="15" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="39"/>
       <c r="C15" s="19">
         <v>2018</v>
@@ -7863,7 +7863,7 @@
       <c r="AP15" s="20"/>
       <c r="AQ15" s="20"/>
     </row>
-    <row r="16" spans="1:43" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="41"/>
       <c r="C16" s="42">
         <v>2021</v>
@@ -7895,12 +7895,12 @@
       <c r="AP16" s="20"/>
       <c r="AQ16" s="20"/>
     </row>
-    <row r="18" spans="1:47" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="59" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:47" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -8197,7 +8197,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -8370,7 +8370,7 @@
       <c r="AT21" s="18"/>
       <c r="AU21" s="18"/>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -8543,24 +8543,24 @@
       <c r="AT22" s="18"/>
       <c r="AU22" s="18"/>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A24" s="59"/>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.3">
       <c r="E28" s="18"/>
     </row>
-    <row r="33" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:21" x14ac:dyDescent="0.3">
       <c r="E33" s="18"/>
     </row>
-    <row r="36" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:21" x14ac:dyDescent="0.3">
       <c r="T36" s="18"/>
       <c r="U36" s="18"/>
     </row>
-    <row r="37" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:21" x14ac:dyDescent="0.3">
       <c r="T37" s="18"/>
       <c r="U37" s="18"/>
     </row>
-    <row r="38" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:21" x14ac:dyDescent="0.3">
       <c r="T38" s="18"/>
       <c r="U38" s="18"/>
     </row>
@@ -8578,33 +8578,33 @@
       <selection pane="bottomLeft" activeCell="A47" sqref="A47:XFD49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="18"/>
-    <col min="2" max="2" width="10.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="18"/>
+    <col min="2" max="2" width="10.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.140625" style="18"/>
-    <col min="16" max="16" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.109375" style="18"/>
+    <col min="16" max="16" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" style="18" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="12" style="18" customWidth="1"/>
-    <col min="20" max="24" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="9.28515625" style="82" customWidth="1"/>
-    <col min="27" max="27" width="11.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.7109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="45" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="46" max="16384" width="9.140625" style="18"/>
+    <col min="20" max="24" width="9.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.33203125" style="82" customWidth="1"/>
+    <col min="27" max="27" width="11.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="30" max="45" width="9.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="46" max="16384" width="9.109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
@@ -8741,7 +8741,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>27</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>29</v>
       </c>
@@ -9008,7 +9008,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>30</v>
       </c>
@@ -9137,7 +9137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>31</v>
       </c>
@@ -9266,7 +9266,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>58</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>59</v>
       </c>
@@ -9524,7 +9524,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="X8" s="20"/>
       <c r="Y8" s="20"/>
       <c r="Z8" s="20"/>
@@ -9547,7 +9547,7 @@
       <c r="AR8" s="20"/>
       <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:45" s="61" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:45" s="61" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="60" t="s">
         <v>110</v>
       </c>
@@ -9573,32 +9573,32 @@
       <c r="AR9" s="62"/>
       <c r="AS9" s="62"/>
     </row>
-    <row r="10" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="63" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="65" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="65" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="65" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="65" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:45" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:45" s="69" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="69" t="s">
         <v>104</v>
       </c>
@@ -9745,7 +9745,7 @@
         <v>3.0466666666666669</v>
       </c>
     </row>
-    <row r="16" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="71" t="s">
         <v>29</v>
       </c>
@@ -9914,7 +9914,7 @@
         <v>658.46820000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="71" t="s">
         <v>30</v>
       </c>
@@ -10062,7 +10062,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="71" t="s">
         <v>31</v>
       </c>
@@ -10210,24 +10210,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:45" s="68" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:45" s="68" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="67"/>
     </row>
-    <row r="21" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:45" s="61" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:45" s="61" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="60" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="63" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:45" s="64" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:45" s="64" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="66"/>
     </row>
-    <row r="25" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="66"/>
       <c r="C25" s="74" t="s">
         <v>103</v>
@@ -10238,7 +10238,7 @@
       <c r="G25" s="61"/>
       <c r="H25" s="75"/>
     </row>
-    <row r="26" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="66"/>
       <c r="C26" s="66"/>
       <c r="D26" s="64" t="s">
@@ -10252,7 +10252,7 @@
       </c>
       <c r="H26" s="76"/>
     </row>
-    <row r="27" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="66"/>
       <c r="C27" s="66"/>
       <c r="D27" s="64" t="s">
@@ -10260,7 +10260,7 @@
       </c>
       <c r="H27" s="76"/>
     </row>
-    <row r="28" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="66"/>
       <c r="C28" s="66"/>
       <c r="D28" s="64">
@@ -10272,7 +10272,7 @@
       </c>
       <c r="H28" s="76"/>
     </row>
-    <row r="29" spans="1:45" s="64" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:45" s="64" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="66"/>
       <c r="C29" s="67"/>
       <c r="D29" s="77" t="s">
@@ -10283,10 +10283,10 @@
       <c r="G29" s="68"/>
       <c r="H29" s="77"/>
     </row>
-    <row r="30" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="66"/>
     </row>
-    <row r="31" spans="1:45" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:45" s="78" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="78" t="s">
         <v>27</v>
       </c>
@@ -10420,7 +10420,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="71" t="s">
         <v>29</v>
       </c>
@@ -10595,7 +10595,7 @@
         <v>658.46820000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="71" t="s">
         <v>30</v>
       </c>
@@ -10771,7 +10771,7 @@
         <v>493.85115000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="71" t="s">
         <v>94</v>
       </c>
@@ -10947,24 +10947,24 @@
         <v>823.08525000000009</v>
       </c>
     </row>
-    <row r="35" spans="1:45" s="68" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:45" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="67"/>
     </row>
-    <row r="36" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:45" s="61" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:45" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:45" s="61" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="60" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="63" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="39" spans="1:45" s="64" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:45" s="64" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="66"/>
     </row>
-    <row r="40" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="66"/>
       <c r="C40" s="60" t="s">
         <v>172</v>
@@ -10975,7 +10975,7 @@
       <c r="G40" s="61"/>
       <c r="H40" s="75"/>
     </row>
-    <row r="41" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="66"/>
       <c r="C41" s="66" t="s">
         <v>173</v>
@@ -10985,7 +10985,7 @@
       </c>
       <c r="H41" s="76"/>
     </row>
-    <row r="42" spans="1:45" s="64" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:45" s="64" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="66"/>
       <c r="C42" s="67"/>
       <c r="D42" s="68"/>
@@ -10994,10 +10994,10 @@
       <c r="G42" s="68"/>
       <c r="H42" s="77"/>
     </row>
-    <row r="43" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="66"/>
     </row>
-    <row r="44" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="66" t="s">
         <v>174</v>
       </c>
@@ -11131,10 +11131,10 @@
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:45" s="64" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="66"/>
     </row>
-    <row r="46" spans="1:45" s="78" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:45" s="78" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="91" t="str">
         <f>A31</f>
         <v>Unit</v>
@@ -11312,7 +11312,7 @@
         <v>euro/m2</v>
       </c>
     </row>
-    <row r="47" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="92" t="str">
         <f t="shared" ref="A47" si="17">A32</f>
         <v>MaxDam</v>
@@ -11494,7 +11494,7 @@
         <v>658.46820000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:45" s="71" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="92" t="str">
         <f t="shared" ref="A48" si="19">A33</f>
         <v>LowerDam</v>
@@ -11676,7 +11676,7 @@
         <v>493.85115000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:45" s="93" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:45" s="93" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="92" t="str">
         <f>A34</f>
         <v>Upperdam</v>
@@ -11858,7 +11858,7 @@
         <v>823.08525000000009</v>
       </c>
     </row>
-    <row r="50" spans="1:45" s="68" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:45" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="67"/>
     </row>
   </sheetData>
@@ -11876,13 +11876,13 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="1" max="1" width="9.109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="44" t="s">
         <v>70</v>
       </c>
@@ -11893,7 +11893,7 @@
       <c r="G2" s="37"/>
       <c r="H2" s="38"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="39"/>
       <c r="C3" s="19" t="s">
         <v>61</v>
@@ -11906,7 +11906,7 @@
       <c r="G3" s="19"/>
       <c r="H3" s="40"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="39" t="s">
         <v>66</v>
       </c>
@@ -11923,7 +11923,7 @@
       <c r="G4" s="19"/>
       <c r="H4" s="40"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="39" t="s">
         <v>67</v>
       </c>
@@ -11940,7 +11940,7 @@
       <c r="G5" s="19"/>
       <c r="H5" s="40"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
         <v>68</v>
       </c>
@@ -11962,7 +11962,7 @@
       </c>
       <c r="H6" s="40"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="39"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -11971,7 +11971,7 @@
       <c r="G7" s="19"/>
       <c r="H7" s="40"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="39"/>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -11980,7 +11980,7 @@
       <c r="G8" s="19"/>
       <c r="H8" s="40"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="39" t="s">
         <v>64</v>
       </c>
@@ -11991,7 +11991,7 @@
       <c r="G9" s="19"/>
       <c r="H9" s="40"/>
     </row>
-    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="41"/>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
@@ -12000,8 +12000,8 @@
       <c r="G10" s="42"/>
       <c r="H10" s="43"/>
     </row>
-    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="44" t="s">
         <v>65</v>
       </c>
@@ -12016,7 +12016,7 @@
       <c r="K14" s="37"/>
       <c r="L14" s="38"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="39"/>
       <c r="C15" s="19" t="s">
         <v>71</v>
@@ -12041,7 +12041,7 @@
       <c r="K15" s="19"/>
       <c r="L15" s="40"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="39" t="s">
         <v>66</v>
       </c>
@@ -12074,7 +12074,7 @@
       <c r="K16" s="19"/>
       <c r="L16" s="40"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="39" t="s">
         <v>67</v>
       </c>
@@ -12112,7 +12112,7 @@
       </c>
       <c r="L17" s="40"/>
     </row>
-    <row r="18" spans="2:12" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="39" t="s">
         <v>69</v>
       </c>
@@ -12150,7 +12150,7 @@
       </c>
       <c r="L18" s="40"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B19" s="39" t="s">
         <v>68</v>
       </c>
@@ -12188,7 +12188,7 @@
       </c>
       <c r="L19" s="40"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="39"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -12201,7 +12201,7 @@
       <c r="K20" s="19"/>
       <c r="L20" s="40"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="39"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -12214,7 +12214,7 @@
       <c r="K21" s="19"/>
       <c r="L21" s="40"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="39" t="s">
         <v>64</v>
       </c>
@@ -12229,7 +12229,7 @@
       <c r="K22" s="19"/>
       <c r="L22" s="40"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="41"/>
       <c r="C23" s="42"/>
       <c r="D23" s="42"/>
@@ -12256,12 +12256,12 @@
       <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1998</v>
       </c>
@@ -12280,7 +12280,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -12304,7 +12304,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -12317,7 +12317,7 @@
       <c r="L5" s="84"/>
       <c r="M5" s="84"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -12330,7 +12330,7 @@
       <c r="L6" s="84"/>
       <c r="M6" s="84"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -12343,7 +12343,7 @@
       <c r="L7" s="84"/>
       <c r="M7" s="84"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -12356,7 +12356,7 @@
       <c r="L8" s="84"/>
       <c r="M8" s="84"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1.5</v>
       </c>
@@ -12369,7 +12369,7 @@
       <c r="L9" s="84"/>
       <c r="M9" s="84"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -12382,7 +12382,7 @@
       <c r="L10" s="84"/>
       <c r="M10" s="84"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -12395,7 +12395,7 @@
       <c r="L11" s="84"/>
       <c r="M11" s="84"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -12408,7 +12408,7 @@
       <c r="L12" s="84"/>
       <c r="M12" s="84"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
@@ -12421,7 +12421,7 @@
       <c r="L13" s="84"/>
       <c r="M13" s="84"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
@@ -12434,17 +12434,17 @@
       <c r="L14" s="84"/>
       <c r="M14" s="84"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K15" s="84"/>
       <c r="L15" s="84"/>
       <c r="M15" s="84"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K16" s="84"/>
       <c r="L16" s="84"/>
       <c r="M16" s="84"/>
     </row>
-    <row r="17" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:13" x14ac:dyDescent="0.3">
       <c r="K17" s="84"/>
       <c r="L17" s="84"/>
       <c r="M17" s="84"/>
@@ -12464,16 +12464,16 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -12484,12 +12484,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="82" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="83" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>120</v>
       </c>
@@ -12500,7 +12500,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="82" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="82" t="s">
         <v>129</v>
       </c>
@@ -12508,7 +12508,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>121</v>
       </c>
@@ -12537,7 +12537,7 @@
         <v>992.09536742754324</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="82" t="s">
         <v>122</v>
       </c>
@@ -12570,7 +12570,7 @@
         <v>1104.8334773624913</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>124</v>
       </c>
@@ -12595,7 +12595,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -12643,7 +12643,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>125</v>
       </c>
@@ -12668,12 +12668,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="83" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>136</v>
       </c>
@@ -12684,7 +12684,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>137</v>
       </c>
@@ -12695,7 +12695,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>138</v>
       </c>
@@ -12706,7 +12706,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>141</v>
       </c>
@@ -12717,7 +12717,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>139</v>
       </c>
@@ -12763,7 +12763,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -12809,12 +12809,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:25" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" s="82" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="82" t="s">
         <v>159</v>
       </c>
@@ -12822,7 +12822,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="22" spans="1:25" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" s="82" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="82" t="s">
         <v>160</v>
       </c>
@@ -12830,8 +12830,8 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="23" spans="1:25" s="82" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" s="82" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -12842,7 +12842,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="J25" s="82" t="s">
         <v>167</v>
       </c>
@@ -12850,7 +12850,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="83" t="s">
         <v>151</v>
       </c>
@@ -12875,7 +12875,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:25" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" s="82" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="83"/>
       <c r="B27" s="82" t="s">
         <v>155</v>
@@ -12920,7 +12920,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>152</v>
       </c>
@@ -12978,7 +12978,7 @@
       </c>
       <c r="Y28" s="82"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>153</v>
       </c>
@@ -13037,7 +13037,7 @@
       <c r="X29" s="82"/>
       <c r="Y29" s="82"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -13096,7 +13096,7 @@
       <c r="X30" s="82"/>
       <c r="Y30" s="82"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="S31">
         <f>AVERAGE(S28:S30)</f>
         <v>11444.578803678598</v>

</xml_diff>